<commit_message>
replacing excel file for format tenaga ahli
</commit_message>
<xml_diff>
--- a/assets/docs/Format Tenaga Ahli.xlsx
+++ b/assets/docs/Format Tenaga Ahli.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vandoc/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6867DF6C-CB3D-D947-BA74-7245D569BD20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A6E5EF-6E1B-1B4C-AA68-7B199981A97F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{5EDCC650-CF7F-BF4C-A922-75EAF64FC947}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kegiatan" sheetId="1" r:id="rId1"/>
+    <sheet name="Tenaga Ahli" sheetId="1" r:id="rId1"/>
     <sheet name="Jenis Kelamin" sheetId="2" r:id="rId2"/>
     <sheet name="Provinsi" sheetId="5" r:id="rId3"/>
     <sheet name="Kota" sheetId="7" r:id="rId4"/>
@@ -2264,7 +2264,7 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>